<commit_message>
627455: Update MCCF tools list - Updated license info
</commit_message>
<xml_diff>
--- a/TASCore_documents/CM/tools_mccf.xlsx
+++ b/TASCore_documents/CM/tools_mccf.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="541">
   <si>
     <t xml:space="preserve">TRM Version </t>
   </si>
@@ -1638,6 +1638,18 @@
   </si>
   <si>
     <t>BCL</t>
+  </si>
+  <si>
+    <t>EPL 1.0</t>
+  </si>
+  <si>
+    <t>ISC License</t>
+  </si>
+  <si>
+    <t>1.1.x, 1.7</t>
+  </si>
+  <si>
+    <t>3.3.x ,3.5.x</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2058,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2056,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4139,6 +4151,9 @@
       <c r="B55" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C55" s="8" t="s">
+        <v>523</v>
+      </c>
       <c r="E55" s="4" t="s">
         <v>110</v>
       </c>
@@ -4177,6 +4192,9 @@
       <c r="B56" s="4" t="s">
         <v>418</v>
       </c>
+      <c r="C56" s="8" t="s">
+        <v>523</v>
+      </c>
       <c r="E56" s="4" t="s">
         <v>511</v>
       </c>
@@ -4215,6 +4233,9 @@
       <c r="B57" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C57" s="8" t="s">
+        <v>522</v>
+      </c>
       <c r="E57" s="4" t="s">
         <v>184</v>
       </c>
@@ -4222,7 +4243,7 @@
         <v>185</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="H57" s="4">
         <v>11497</v>
@@ -4253,6 +4274,9 @@
       <c r="B58" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C58" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="E58" s="4" t="s">
         <v>87</v>
       </c>
@@ -4260,7 +4284,7 @@
         <v>88</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="H58" s="4">
         <v>11176</v>
@@ -4291,6 +4315,9 @@
       <c r="B59" s="4" t="s">
         <v>361</v>
       </c>
+      <c r="C59" s="8" t="s">
+        <v>537</v>
+      </c>
       <c r="E59" s="4">
         <v>4.12</v>
       </c>
@@ -4329,6 +4356,9 @@
       <c r="B60" s="4" t="s">
         <v>361</v>
       </c>
+      <c r="C60" s="8" t="s">
+        <v>538</v>
+      </c>
       <c r="E60" s="4" t="s">
         <v>368</v>
       </c>
@@ -4336,7 +4366,7 @@
         <v>54</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="H60" s="4">
         <v>11181</v>
@@ -4367,14 +4397,17 @@
       <c r="B61" s="4" t="s">
         <v>418</v>
       </c>
+      <c r="C61" s="8" t="s">
+        <v>523</v>
+      </c>
       <c r="E61" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>100</v>
+        <v>539</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="H61" s="4">
         <v>8882</v>
@@ -4398,79 +4431,85 @@
         <v>454</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="C62" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="10">
         <v>7402</v>
       </c>
-      <c r="I62" s="6">
+      <c r="I62" s="11">
         <v>42888</v>
       </c>
-      <c r="J62" s="6">
+      <c r="J62" s="11">
         <v>43038</v>
       </c>
-      <c r="K62" s="6">
+      <c r="K62" s="11">
         <v>42962</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L62" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="M62" t="s">
+      <c r="M62" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="10">
         <v>2.8</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="G63" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H63" s="10">
         <v>6710</v>
       </c>
-      <c r="I63" s="6">
+      <c r="I63" s="11">
         <v>42620</v>
       </c>
-      <c r="J63" s="6">
+      <c r="J63" s="11">
         <v>43038</v>
       </c>
-      <c r="K63" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L63" t="s">
+      <c r="K63" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L63" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M63" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N63" s="9" t="s">
         <v>404</v>
       </c>
     </row>
@@ -4481,14 +4520,17 @@
       <c r="B64" s="4" t="s">
         <v>313</v>
       </c>
+      <c r="C64" s="8" t="s">
+        <v>522</v>
+      </c>
       <c r="E64" s="4" t="s">
         <v>355</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>142</v>
+        <v>540</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="H64" s="4">
         <v>1101</v>
@@ -6148,8 +6190,17 @@
     <hyperlink ref="C52" r:id="rId33"/>
     <hyperlink ref="C53" r:id="rId34"/>
     <hyperlink ref="C54" r:id="rId35"/>
+    <hyperlink ref="C55" r:id="rId36"/>
+    <hyperlink ref="C56" r:id="rId37"/>
+    <hyperlink ref="C57" r:id="rId38"/>
+    <hyperlink ref="C58" r:id="rId39"/>
+    <hyperlink ref="C59" r:id="rId40"/>
+    <hyperlink ref="C60" r:id="rId41"/>
+    <hyperlink ref="C61" r:id="rId42"/>
+    <hyperlink ref="C62" r:id="rId43"/>
+    <hyperlink ref="C64" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>